<commit_message>
Updated ITA model - 2025-07-28 21:07
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C70BD67-059F-4F50-A8DB-CD30DBCA57A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B6B18-7997-4B40-826B-F8F4C70DAEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="historical_data" sheetId="4" r:id="rId1"/>
-    <sheet name="Veda" sheetId="1" r:id="rId2"/>
-    <sheet name="iamc_data" sheetId="2" r:id="rId3"/>
-    <sheet name="base_year_data" sheetId="3" r:id="rId4"/>
+    <sheet name="Veda" sheetId="1" r:id="rId1"/>
+    <sheet name="iamc_data" sheetId="2" r:id="rId2"/>
+    <sheet name="historical_data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="54">
   <si>
     <t>~Inputcell: 3</t>
   </si>
@@ -107,9 +106,6 @@
     <t>Downscaling[MESSAGEix-GLOBIOM 1.1-M-R12]</t>
   </si>
   <si>
-    <t>MEX</t>
-  </si>
-  <si>
     <t>Final Energy|Industry|Electricity</t>
   </si>
   <si>
@@ -183,9 +179,6 @@
   </si>
   <si>
     <t>hydro</t>
-  </si>
-  <si>
-    <t>nuclear</t>
   </si>
   <si>
     <t>solar</t>
@@ -210,7 +203,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,11 +217,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
     </font>
     <font>
       <sz val="11"/>
@@ -276,27 +264,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -330,21 +303,18 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -682,226 +652,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0B791C-0A90-43EF-923A-A4B5B9D728EB}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2">
-        <v>3.1</v>
-      </c>
-      <c r="D2">
-        <v>3.3</v>
-      </c>
-      <c r="E2">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="F2">
-        <v>23.5</v>
-      </c>
-      <c r="G2">
-        <v>0.59</v>
-      </c>
-      <c r="H2">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3">
-        <v>17.2</v>
-      </c>
-      <c r="F3">
-        <v>22.6</v>
-      </c>
-      <c r="H3">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4">
-        <v>111.9</v>
-      </c>
-      <c r="F4">
-        <v>141.5</v>
-      </c>
-      <c r="H4">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5">
-        <v>6.3</v>
-      </c>
-      <c r="E5">
-        <v>5.8</v>
-      </c>
-      <c r="G5">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6">
-        <v>20.7</v>
-      </c>
-      <c r="D6">
-        <v>23.4</v>
-      </c>
-      <c r="E6">
-        <v>30.3</v>
-      </c>
-      <c r="F6">
-        <v>28.4</v>
-      </c>
-      <c r="G6">
-        <v>0.15</v>
-      </c>
-      <c r="H6">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7">
-        <v>0.6</v>
-      </c>
-      <c r="D7">
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>15.6</v>
-      </c>
-      <c r="G7">
-        <v>0.03</v>
-      </c>
-      <c r="H7">
-        <v>1.24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8">
-        <v>5.4</v>
-      </c>
-      <c r="D8">
-        <v>5.4</v>
-      </c>
-      <c r="E8">
-        <v>28.1</v>
-      </c>
-      <c r="F8">
-        <v>28.1</v>
-      </c>
-      <c r="G8">
-        <v>0.13</v>
-      </c>
-      <c r="H8">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9">
-        <v>17</v>
-      </c>
-      <c r="D9">
-        <v>16.8</v>
-      </c>
-      <c r="E9">
-        <v>20.5</v>
-      </c>
-      <c r="F9">
-        <v>20.3</v>
-      </c>
-      <c r="G9">
-        <v>0.2</v>
-      </c>
-      <c r="H9">
-        <v>0.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA19"/>
   <sheetViews>
@@ -967,12 +717,12 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="Q10" s="5">
-        <f>SUM(base_year_data!F2:F16)</f>
-        <v>340.2</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>54</v>
+      <c r="Q10" s="4">
+        <f>SUM(historical_data!F2:F16)</f>
+        <v>280</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:27" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
@@ -1000,7 +750,7 @@
       </c>
     </row>
     <row r="14" spans="2:27" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="Q14" s="7" t="s">
+      <c r="Q14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1033,31 +783,31 @@
         <f>iamc_data!L1</f>
         <v>2050</v>
       </c>
-      <c r="Q15" s="6" t="s">
+      <c r="Q15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15" s="5">
         <v>2022</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="5">
         <v>2025</v>
       </c>
-      <c r="T15" s="6">
+      <c r="T15" s="5">
         <v>2030</v>
       </c>
-      <c r="U15" s="6">
+      <c r="U15" s="5">
         <v>2035</v>
       </c>
-      <c r="V15" s="6">
+      <c r="V15" s="5">
         <v>2040</v>
       </c>
-      <c r="W15" s="6">
+      <c r="W15" s="5">
         <v>2045</v>
       </c>
-      <c r="X15" s="6">
+      <c r="X15" s="5">
         <v>2050</v>
       </c>
-      <c r="Y15" s="6" t="s">
+      <c r="Y15" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1095,37 +845,37 @@
       </c>
       <c r="R16" s="1">
         <f>$Q$10*G16/SUM($G$16:$G$18)</f>
-        <v>16.412233336283968</v>
+        <v>13.508010976365405</v>
       </c>
       <c r="S16" s="1">
         <f>R16</f>
-        <v>16.412233336283968</v>
+        <v>13.508010976365405</v>
       </c>
       <c r="T16" s="1">
         <f t="shared" ref="T16:X16" si="0">S16</f>
-        <v>16.412233336283968</v>
+        <v>13.508010976365405</v>
       </c>
       <c r="U16" s="1">
         <f t="shared" si="0"/>
-        <v>16.412233336283968</v>
+        <v>13.508010976365405</v>
       </c>
       <c r="V16" s="1">
         <f t="shared" si="0"/>
-        <v>16.412233336283968</v>
+        <v>13.508010976365405</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="0"/>
-        <v>16.412233336283968</v>
+        <v>13.508010976365405</v>
       </c>
       <c r="X16" s="1">
         <f t="shared" si="0"/>
-        <v>16.412233336283968</v>
+        <v>13.508010976365405</v>
       </c>
       <c r="Y16" t="s">
         <v>12</v>
       </c>
-      <c r="AA16" s="4" t="s">
-        <v>53</v>
+      <c r="AA16" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="7:25" x14ac:dyDescent="0.45">
@@ -1162,31 +912,31 @@
       </c>
       <c r="R17" s="1">
         <f>$Q$10*G17/SUM($G$16:$G$18)</f>
-        <v>210.28738603168981</v>
+        <v>173.07603788616444</v>
       </c>
       <c r="S17" s="1">
         <f t="shared" ref="S17:X18" si="1">R17*H17/G17</f>
-        <v>244.67779056386647</v>
+        <v>201.38089758342917</v>
       </c>
       <c r="T17" s="1">
         <f t="shared" si="1"/>
-        <v>265.36623882446662</v>
+        <v>218.4084270160219</v>
       </c>
       <c r="U17" s="1">
         <f t="shared" si="1"/>
-        <v>275.27380720545273</v>
+        <v>226.56280428432322</v>
       </c>
       <c r="V17" s="1">
         <f t="shared" si="1"/>
-        <v>290.48147295742228</v>
+        <v>239.07940161104713</v>
       </c>
       <c r="W17" s="1">
         <f t="shared" si="1"/>
-        <v>307.46587589625557</v>
+        <v>253.0583340709922</v>
       </c>
       <c r="X17" s="1">
         <f t="shared" si="1"/>
-        <v>330.89471541117103</v>
+        <v>272.34132955651938</v>
       </c>
       <c r="Y17" t="s">
         <v>12</v>
@@ -1226,31 +976,31 @@
       </c>
       <c r="R18" s="1">
         <f>$Q$10*G18/SUM($G$16:$G$18)</f>
-        <v>113.50038063202619</v>
+        <v>93.415951137470117</v>
       </c>
       <c r="S18" s="1">
         <f t="shared" si="1"/>
-        <v>97.208604054173648</v>
+        <v>80.007081526068859</v>
       </c>
       <c r="T18" s="1">
         <f t="shared" si="1"/>
-        <v>88.595945826325561</v>
+        <v>72.918473931132169</v>
       </c>
       <c r="U18" s="1">
         <f t="shared" si="1"/>
-        <v>84.048703195538621</v>
+        <v>69.175887403735516</v>
       </c>
       <c r="V18" s="1">
         <f t="shared" si="1"/>
-        <v>82.302080198282709</v>
+        <v>67.738337611755341</v>
       </c>
       <c r="W18" s="1">
         <f t="shared" si="1"/>
-        <v>82.964592369655648</v>
+        <v>68.283615119058169</v>
       </c>
       <c r="X18" s="1">
         <f t="shared" si="1"/>
-        <v>90.974966805346526</v>
+        <v>74.876515889174129</v>
       </c>
       <c r="Y18" t="s">
         <v>12</v>
@@ -1258,7 +1008,7 @@
     </row>
     <row r="19" spans="7:25" x14ac:dyDescent="0.45">
       <c r="Q19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R19" s="1">
         <f>$Q$10*G16/SUM($G$16:$G$18)-R16</f>
@@ -1266,27 +1016,27 @@
       </c>
       <c r="S19" s="1">
         <f t="shared" ref="S19:X19" si="2">$Q$10*H16/SUM($G$16:$G$18)-S16</f>
-        <v>-3.914844649021866</v>
+        <v>-3.2220943613348663</v>
       </c>
       <c r="T19" s="1">
         <f t="shared" si="2"/>
-        <v>-1.0539966362751212</v>
+        <v>-0.86748694343631172</v>
       </c>
       <c r="U19" s="1">
         <f t="shared" si="2"/>
-        <v>6.4444365760821434</v>
+        <v>5.3040630255820105</v>
       </c>
       <c r="V19" s="1">
         <f t="shared" si="2"/>
-        <v>21.802673276090999</v>
+        <v>17.944587058511111</v>
       </c>
       <c r="W19" s="1">
         <f t="shared" si="2"/>
-        <v>53.151544657873764</v>
+        <v>43.74612729043109</v>
       </c>
       <c r="X19" s="1">
         <f t="shared" si="2"/>
-        <v>86.277153226520312</v>
+        <v>71.010002655572265</v>
       </c>
       <c r="Y19" t="s">
         <v>12</v>
@@ -1297,11 +1047,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -1360,13 +1110,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
       </c>
       <c r="F2">
         <v>0.37469999999999998</v>
@@ -1390,10 +1140,10 @@
         <v>0.32619999999999999</v>
       </c>
       <c r="M2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
         <v>14</v>
@@ -1407,13 +1157,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
       </c>
       <c r="F3">
         <v>0.37209999999999999</v>
@@ -1437,10 +1187,10 @@
         <v>0.40739999999999998</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
         <v>14</v>
@@ -1454,13 +1204,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>5.45E-2</v>
@@ -1484,10 +1234,10 @@
         <v>0.34100000000000003</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O4" t="s">
         <v>11</v>
@@ -1501,13 +1251,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>0.69830000000000003</v>
@@ -1531,10 +1281,10 @@
         <v>1.0988</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O5" t="s">
         <v>13</v>
@@ -1548,13 +1298,13 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
       </c>
       <c r="F6">
         <v>0.37690000000000001</v>
@@ -1578,10 +1328,10 @@
         <v>0.30209999999999998</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O6" t="s">
         <v>14</v>
@@ -1595,13 +1345,13 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
       </c>
       <c r="F7">
         <v>0.37359999999999999</v>
@@ -1625,10 +1375,10 @@
         <v>0.32779999999999998</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O7" t="s">
         <v>14</v>
@@ -1642,13 +1392,13 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>0.69940000000000002</v>
@@ -1672,10 +1422,10 @@
         <v>1.2003999999999999</v>
       </c>
       <c r="M8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O8" t="s">
         <v>13</v>
@@ -1689,13 +1439,13 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>5.1999999999999998E-2</v>
@@ -1719,10 +1469,10 @@
         <v>0.36030000000000001</v>
       </c>
       <c r="M9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O9" t="s">
         <v>11</v>
@@ -1736,13 +1486,13 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10">
         <v>6.3399999999999998E-2</v>
@@ -1766,10 +1516,10 @@
         <v>6.4799999999999996E-2</v>
       </c>
       <c r="M10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O10" t="s">
         <v>11</v>
@@ -1783,13 +1533,13 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>0.69110000000000005</v>
@@ -1813,10 +1563,10 @@
         <v>1.4702999999999999</v>
       </c>
       <c r="M11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O11" t="s">
         <v>13</v>
@@ -1830,13 +1580,13 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
         <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
       </c>
       <c r="F12">
         <v>0.37469999999999998</v>
@@ -1860,10 +1610,10 @@
         <v>0.25719999999999998</v>
       </c>
       <c r="M12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O12" t="s">
         <v>14</v>
@@ -1877,13 +1627,13 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13">
         <v>0.68179999999999996</v>
@@ -1907,10 +1657,10 @@
         <v>1.1176999999999999</v>
       </c>
       <c r="M13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O13" t="s">
         <v>13</v>
@@ -1924,13 +1674,13 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14">
         <v>5.2699999999999997E-2</v>
@@ -1954,10 +1704,10 @@
         <v>0.2424</v>
       </c>
       <c r="M14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O14" t="s">
         <v>11</v>
@@ -1971,13 +1721,13 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15">
         <v>0.67979999999999996</v>
@@ -2001,10 +1751,10 @@
         <v>1.3542000000000001</v>
       </c>
       <c r="M15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O15" t="s">
         <v>13</v>
@@ -2018,13 +1768,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
         <v>24</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
       </c>
       <c r="F16">
         <v>0.38769999999999999</v>
@@ -2048,10 +1798,10 @@
         <v>0.25390000000000001</v>
       </c>
       <c r="M16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O16" t="s">
         <v>14</v>
@@ -2065,13 +1815,13 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17">
         <v>5.5100000000000003E-2</v>
@@ -2095,10 +1845,10 @@
         <v>0.36180000000000001</v>
       </c>
       <c r="M17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O17" t="s">
         <v>11</v>
@@ -2112,13 +1862,13 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <v>0.69269999999999998</v>
@@ -2142,10 +1892,10 @@
         <v>1.1363000000000001</v>
       </c>
       <c r="M18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O18" t="s">
         <v>13</v>
@@ -2159,13 +1909,13 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
         <v>24</v>
-      </c>
-      <c r="E19" t="s">
-        <v>25</v>
       </c>
       <c r="F19">
         <v>0.37440000000000001</v>
@@ -2189,10 +1939,10 @@
         <v>0.3271</v>
       </c>
       <c r="M19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O19" t="s">
         <v>14</v>
@@ -2206,13 +1956,13 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F20">
         <v>0.69920000000000004</v>
@@ -2236,10 +1986,10 @@
         <v>0.78369999999999995</v>
       </c>
       <c r="M20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O20" t="s">
         <v>13</v>
@@ -2253,13 +2003,13 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F21">
         <v>5.8999999999999997E-2</v>
@@ -2283,10 +2033,10 @@
         <v>0.44130000000000003</v>
       </c>
       <c r="M21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O21" t="s">
         <v>11</v>
@@ -2300,13 +2050,13 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22">
         <v>6.4100000000000004E-2</v>
@@ -2330,10 +2080,10 @@
         <v>0.35870000000000002</v>
       </c>
       <c r="M22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O22" t="s">
         <v>11</v>
@@ -2347,13 +2097,13 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
         <v>29</v>
-      </c>
-      <c r="E23" t="s">
-        <v>30</v>
       </c>
       <c r="F23">
         <v>0.79330000000000001</v>
@@ -2377,13 +2127,13 @@
         <v>41.091099999999997</v>
       </c>
       <c r="M23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N23" t="s">
+        <v>30</v>
+      </c>
+      <c r="O23" t="s">
         <v>31</v>
-      </c>
-      <c r="O23" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
@@ -2394,13 +2144,13 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24">
         <v>1.8210999999999999</v>
@@ -2424,13 +2174,13 @@
         <v>10.4336</v>
       </c>
       <c r="M24" t="s">
+        <v>32</v>
+      </c>
+      <c r="N24" t="s">
+        <v>30</v>
+      </c>
+      <c r="O24" t="s">
         <v>33</v>
-      </c>
-      <c r="N24" t="s">
-        <v>31</v>
-      </c>
-      <c r="O24" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
@@ -2441,13 +2191,13 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25">
         <v>2.4039000000000001</v>
@@ -2471,13 +2221,13 @@
         <v>7.3807999999999998</v>
       </c>
       <c r="M25" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" t="s">
         <v>35</v>
-      </c>
-      <c r="N25" t="s">
-        <v>31</v>
-      </c>
-      <c r="O25" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
@@ -2488,13 +2238,13 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26">
         <v>2.4039000000000001</v>
@@ -2518,13 +2268,13 @@
         <v>4.7949000000000002</v>
       </c>
       <c r="M26" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" t="s">
+        <v>30</v>
+      </c>
+      <c r="O26" t="s">
         <v>35</v>
-      </c>
-      <c r="N26" t="s">
-        <v>31</v>
-      </c>
-      <c r="O26" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
@@ -2535,13 +2285,13 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27">
         <v>1.8210999999999999</v>
@@ -2565,13 +2315,13 @@
         <v>6.3018999999999998</v>
       </c>
       <c r="M27" t="s">
+        <v>32</v>
+      </c>
+      <c r="N27" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" t="s">
         <v>33</v>
-      </c>
-      <c r="N27" t="s">
-        <v>31</v>
-      </c>
-      <c r="O27" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
@@ -2582,13 +2332,13 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28">
         <v>3.1242999999999999</v>
@@ -2612,13 +2362,13 @@
         <v>5.2706</v>
       </c>
       <c r="M28" t="s">
+        <v>36</v>
+      </c>
+      <c r="N28" t="s">
+        <v>30</v>
+      </c>
+      <c r="O28" t="s">
         <v>37</v>
-      </c>
-      <c r="N28" t="s">
-        <v>31</v>
-      </c>
-      <c r="O28" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
@@ -2629,13 +2379,13 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
         <v>29</v>
-      </c>
-      <c r="E29" t="s">
-        <v>30</v>
       </c>
       <c r="F29">
         <v>0.79330000000000001</v>
@@ -2659,13 +2409,13 @@
         <v>9.2622999999999998</v>
       </c>
       <c r="M29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N29" t="s">
+        <v>30</v>
+      </c>
+      <c r="O29" t="s">
         <v>31</v>
-      </c>
-      <c r="O29" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
@@ -2676,13 +2426,13 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30">
         <v>1.8210999999999999</v>
@@ -2706,13 +2456,13 @@
         <v>2.6432000000000002</v>
       </c>
       <c r="M30" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30" t="s">
+        <v>30</v>
+      </c>
+      <c r="O30" t="s">
         <v>33</v>
-      </c>
-      <c r="N30" t="s">
-        <v>31</v>
-      </c>
-      <c r="O30" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
@@ -2723,13 +2473,13 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31">
         <v>3.1242999999999999</v>
@@ -2753,13 +2503,13 @@
         <v>4.6989999999999998</v>
       </c>
       <c r="M31" t="s">
+        <v>36</v>
+      </c>
+      <c r="N31" t="s">
+        <v>30</v>
+      </c>
+      <c r="O31" t="s">
         <v>37</v>
-      </c>
-      <c r="N31" t="s">
-        <v>31</v>
-      </c>
-      <c r="O31" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
@@ -2770,13 +2520,13 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
         <v>29</v>
-      </c>
-      <c r="E32" t="s">
-        <v>30</v>
       </c>
       <c r="F32">
         <v>0.79330000000000001</v>
@@ -2800,13 +2550,13 @@
         <v>18.1554</v>
       </c>
       <c r="M32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N32" t="s">
+        <v>30</v>
+      </c>
+      <c r="O32" t="s">
         <v>31</v>
-      </c>
-      <c r="O32" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.45">
@@ -2817,13 +2567,13 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
         <v>29</v>
-      </c>
-      <c r="E33" t="s">
-        <v>30</v>
       </c>
       <c r="F33">
         <v>0.79330000000000001</v>
@@ -2847,13 +2597,13 @@
         <v>6.9612999999999996</v>
       </c>
       <c r="M33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N33" t="s">
+        <v>30</v>
+      </c>
+      <c r="O33" t="s">
         <v>31</v>
-      </c>
-      <c r="O33" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
@@ -2864,13 +2614,13 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34">
         <v>2.4039000000000001</v>
@@ -2894,13 +2644,13 @@
         <v>4.7228000000000003</v>
       </c>
       <c r="M34" t="s">
+        <v>34</v>
+      </c>
+      <c r="N34" t="s">
+        <v>30</v>
+      </c>
+      <c r="O34" t="s">
         <v>35</v>
-      </c>
-      <c r="N34" t="s">
-        <v>31</v>
-      </c>
-      <c r="O34" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
@@ -2911,13 +2661,13 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
         <v>29</v>
-      </c>
-      <c r="E35" t="s">
-        <v>30</v>
       </c>
       <c r="F35">
         <v>0.79330000000000001</v>
@@ -2941,13 +2691,13 @@
         <v>11.804</v>
       </c>
       <c r="M35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N35" t="s">
+        <v>30</v>
+      </c>
+      <c r="O35" t="s">
         <v>31</v>
-      </c>
-      <c r="O35" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.45">
@@ -2958,13 +2708,13 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36">
         <v>1.8210999999999999</v>
@@ -2988,13 +2738,13 @@
         <v>3.4154</v>
       </c>
       <c r="M36" t="s">
+        <v>32</v>
+      </c>
+      <c r="N36" t="s">
+        <v>30</v>
+      </c>
+      <c r="O36" t="s">
         <v>33</v>
-      </c>
-      <c r="N36" t="s">
-        <v>31</v>
-      </c>
-      <c r="O36" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.45">
@@ -3005,13 +2755,13 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F37">
         <v>2.4039000000000001</v>
@@ -3035,13 +2785,13 @@
         <v>4.9874000000000001</v>
       </c>
       <c r="M37" t="s">
+        <v>34</v>
+      </c>
+      <c r="N37" t="s">
+        <v>30</v>
+      </c>
+      <c r="O37" t="s">
         <v>35</v>
-      </c>
-      <c r="N37" t="s">
-        <v>31</v>
-      </c>
-      <c r="O37" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
@@ -3052,13 +2802,13 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F38">
         <v>3.1242999999999999</v>
@@ -3082,13 +2832,13 @@
         <v>4.5690999999999997</v>
       </c>
       <c r="M38" t="s">
+        <v>36</v>
+      </c>
+      <c r="N38" t="s">
+        <v>30</v>
+      </c>
+      <c r="O38" t="s">
         <v>37</v>
-      </c>
-      <c r="N38" t="s">
-        <v>31</v>
-      </c>
-      <c r="O38" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
@@ -3099,13 +2849,13 @@
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
         <v>29</v>
-      </c>
-      <c r="E39" t="s">
-        <v>30</v>
       </c>
       <c r="F39">
         <v>0.79330000000000001</v>
@@ -3129,13 +2879,13 @@
         <v>12.6198</v>
       </c>
       <c r="M39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N39" t="s">
+        <v>30</v>
+      </c>
+      <c r="O39" t="s">
         <v>31</v>
-      </c>
-      <c r="O39" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
@@ -3146,13 +2896,13 @@
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F40">
         <v>1.8210999999999999</v>
@@ -3176,13 +2926,13 @@
         <v>2.7033</v>
       </c>
       <c r="M40" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" t="s">
         <v>33</v>
-      </c>
-      <c r="N40" t="s">
-        <v>31</v>
-      </c>
-      <c r="O40" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.45">
@@ -3193,13 +2943,13 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F41">
         <v>3.1242999999999999</v>
@@ -3223,13 +2973,13 @@
         <v>5.7683</v>
       </c>
       <c r="M41" t="s">
+        <v>36</v>
+      </c>
+      <c r="N41" t="s">
+        <v>30</v>
+      </c>
+      <c r="O41" t="s">
         <v>37</v>
-      </c>
-      <c r="N41" t="s">
-        <v>31</v>
-      </c>
-      <c r="O41" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
@@ -3240,13 +2990,13 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42">
         <v>2.4039000000000001</v>
@@ -3270,13 +3020,13 @@
         <v>4.8583999999999996</v>
       </c>
       <c r="M42" t="s">
+        <v>34</v>
+      </c>
+      <c r="N42" t="s">
+        <v>30</v>
+      </c>
+      <c r="O42" t="s">
         <v>35</v>
-      </c>
-      <c r="N42" t="s">
-        <v>31</v>
-      </c>
-      <c r="O42" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.45">
@@ -3287,13 +3037,13 @@
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
         <v>29</v>
-      </c>
-      <c r="E43" t="s">
-        <v>30</v>
       </c>
       <c r="F43">
         <v>0.79330000000000001</v>
@@ -3317,13 +3067,13 @@
         <v>3.1745000000000001</v>
       </c>
       <c r="M43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" t="s">
         <v>31</v>
-      </c>
-      <c r="O43" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.45">
@@ -3334,13 +3084,13 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F44">
         <v>1.8210999999999999</v>
@@ -3364,13 +3114,13 @@
         <v>2.6608999999999998</v>
       </c>
       <c r="M44" t="s">
+        <v>32</v>
+      </c>
+      <c r="N44" t="s">
+        <v>30</v>
+      </c>
+      <c r="O44" t="s">
         <v>33</v>
-      </c>
-      <c r="N44" t="s">
-        <v>31</v>
-      </c>
-      <c r="O44" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.45">
@@ -3381,13 +3131,13 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F45">
         <v>2.4039000000000001</v>
@@ -3411,13 +3161,13 @@
         <v>4.7777000000000003</v>
       </c>
       <c r="M45" t="s">
+        <v>34</v>
+      </c>
+      <c r="N45" t="s">
+        <v>30</v>
+      </c>
+      <c r="O45" t="s">
         <v>35</v>
-      </c>
-      <c r="N45" t="s">
-        <v>31</v>
-      </c>
-      <c r="O45" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
@@ -3428,13 +3178,13 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F46">
         <v>3.1242999999999999</v>
@@ -3458,13 +3208,13 @@
         <v>6.5091999999999999</v>
       </c>
       <c r="M46" t="s">
+        <v>36</v>
+      </c>
+      <c r="N46" t="s">
+        <v>30</v>
+      </c>
+      <c r="O46" t="s">
         <v>37</v>
-      </c>
-      <c r="N46" t="s">
-        <v>31</v>
-      </c>
-      <c r="O46" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
@@ -3475,13 +3225,13 @@
         <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F47">
         <v>2.4039000000000001</v>
@@ -3505,13 +3255,13 @@
         <v>5.2603999999999997</v>
       </c>
       <c r="M47" t="s">
+        <v>34</v>
+      </c>
+      <c r="N47" t="s">
+        <v>30</v>
+      </c>
+      <c r="O47" t="s">
         <v>35</v>
-      </c>
-      <c r="N47" t="s">
-        <v>31</v>
-      </c>
-      <c r="O47" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
@@ -3522,13 +3272,13 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F48">
         <v>1.8210999999999999</v>
@@ -3552,13 +3302,13 @@
         <v>2.1049000000000002</v>
       </c>
       <c r="M48" t="s">
+        <v>32</v>
+      </c>
+      <c r="N48" t="s">
+        <v>30</v>
+      </c>
+      <c r="O48" t="s">
         <v>33</v>
-      </c>
-      <c r="N48" t="s">
-        <v>31</v>
-      </c>
-      <c r="O48" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.45">
@@ -3569,13 +3319,13 @@
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F49">
         <v>3.1242999999999999</v>
@@ -3599,13 +3349,13 @@
         <v>5.8238000000000003</v>
       </c>
       <c r="M49" t="s">
+        <v>36</v>
+      </c>
+      <c r="N49" t="s">
+        <v>30</v>
+      </c>
+      <c r="O49" t="s">
         <v>37</v>
-      </c>
-      <c r="N49" t="s">
-        <v>31</v>
-      </c>
-      <c r="O49" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.45">
@@ -3616,13 +3366,13 @@
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F50">
         <v>3.1242999999999999</v>
@@ -3646,13 +3396,13 @@
         <v>3.1471</v>
       </c>
       <c r="M50" t="s">
+        <v>36</v>
+      </c>
+      <c r="N50" t="s">
+        <v>30</v>
+      </c>
+      <c r="O50" t="s">
         <v>37</v>
-      </c>
-      <c r="N50" t="s">
-        <v>31</v>
-      </c>
-      <c r="O50" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3660,9 +3410,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
@@ -3680,254 +3430,210 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>0.7</v>
+        <v>3.1</v>
       </c>
       <c r="D2">
-        <v>2.4</v>
+        <v>3.3</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F2">
-        <v>6.7</v>
+        <v>23.5</v>
       </c>
       <c r="G2">
-        <v>0.26</v>
+        <v>0.59</v>
       </c>
       <c r="H2">
-        <v>0.88</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3">
-        <v>21.5</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>21.4</v>
-      </c>
-      <c r="E3">
-        <v>24</v>
+        <v>17.2</v>
       </c>
       <c r="F3">
-        <v>21.4</v>
-      </c>
-      <c r="G3">
-        <v>0.46</v>
+        <v>22.6</v>
       </c>
       <c r="H3">
-        <v>0.45</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4">
-        <v>257.3</v>
+        <v>35</v>
       </c>
       <c r="D4">
-        <v>192.6</v>
-      </c>
-      <c r="E4">
-        <v>217.5</v>
+        <v>111.9</v>
       </c>
       <c r="F4">
-        <v>192.1</v>
-      </c>
-      <c r="G4">
-        <v>0.67</v>
+        <v>141.5</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5">
-        <v>4.3</v>
+        <v>6.3</v>
       </c>
       <c r="E5">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="G5">
-        <v>0.52</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6">
-        <v>33</v>
+        <v>20.7</v>
       </c>
       <c r="D6">
-        <v>31.6</v>
+        <v>23.4</v>
       </c>
       <c r="E6">
-        <v>35.9</v>
+        <v>30.3</v>
       </c>
       <c r="F6">
-        <v>35.6</v>
+        <v>28.4</v>
       </c>
       <c r="G6">
-        <v>0.32</v>
+        <v>0.15</v>
       </c>
       <c r="H6">
-        <v>0.31</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C7">
-        <v>10.8</v>
+        <v>0.6</v>
       </c>
       <c r="D7">
-        <v>10.8</v>
+        <v>24</v>
       </c>
       <c r="E7">
-        <v>10.9</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>10.9</v>
+        <v>15.6</v>
       </c>
       <c r="G7">
-        <v>0.77</v>
+        <v>0.03</v>
       </c>
       <c r="H7">
-        <v>0.77</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C8">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="D8">
-        <v>8.4</v>
+        <v>5.4</v>
       </c>
       <c r="E8">
-        <v>39.799999999999997</v>
+        <v>28.1</v>
       </c>
       <c r="F8">
-        <v>32.700000000000003</v>
+        <v>28.1</v>
       </c>
       <c r="G8">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="H8">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9">
-        <v>28.2</v>
+        <v>17</v>
       </c>
       <c r="D9">
-        <v>27.9</v>
+        <v>16.8</v>
       </c>
       <c r="E9">
-        <v>20.6</v>
+        <v>20.5</v>
       </c>
       <c r="F9">
         <v>20.3</v>
       </c>
       <c r="G9">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="H9">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10">
-        <v>22.3</v>
-      </c>
-      <c r="D10">
-        <v>23.1</v>
-      </c>
-      <c r="E10">
-        <v>20.6</v>
-      </c>
-      <c r="F10">
-        <v>20.5</v>
-      </c>
-      <c r="G10">
-        <v>0.31</v>
-      </c>
-      <c r="H10">
-        <v>0.32</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-07 13:45
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_ITA/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CED64BDB-8682-4265-90B1-E14733D6B325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DE9DB6C-2925-4E7A-B8BF-47CAA433F8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -753,25 +753,25 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>322.95000000000005</c:v>
+                  <c:v>279.96000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>344.28967318510593</c:v>
+                  <c:v>298.45900884007506</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>387.25739351727844</c:v>
+                  <c:v>335.707013126172</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>381.86480042860984</c:v>
+                  <c:v>331.03226359496387</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>377.02011786766684</c:v>
+                  <c:v>326.8324886150549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>386.96901955531752</c:v>
+                  <c:v>335.45702652022504</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>415.17199303509244</c:v>
+                  <c:v>359.90571658183768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2783,7 +2783,7 @@
   <dimension ref="B2:AA34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2852,8 +2852,8 @@
         <v>3</v>
       </c>
       <c r="Q10" s="3">
-        <f>SUMIFS(historical_data_long!$D$3:$D$9999,historical_data_long!$B$3:$B$9999,Veda!Q9,historical_data_long!$C$3:$C$9999,"TWh")</f>
-        <v>322.95000000000005</v>
+        <f>SUMIFS(historical_data_long!$D$3:$D$9999,historical_data_long!$B$3:$B$9999,Veda!Q9,historical_data_long!$C$3:$C$9999,"TWh")-R25+R26</f>
+        <v>279.96000000000004</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>16</v>
@@ -2876,31 +2876,31 @@
       </c>
       <c r="R12" s="8">
         <f>SUM(R16:R19)</f>
-        <v>322.95000000000005</v>
+        <v>279.96000000000004</v>
       </c>
       <c r="S12" s="8">
         <f t="shared" ref="S12:X12" si="0">SUM(S16:S19)</f>
-        <v>344.28967318510593</v>
+        <v>298.45900884007506</v>
       </c>
       <c r="T12" s="8">
         <f t="shared" si="0"/>
-        <v>387.25739351727844</v>
+        <v>335.707013126172</v>
       </c>
       <c r="U12" s="8">
         <f t="shared" si="0"/>
-        <v>381.86480042860984</v>
+        <v>331.03226359496387</v>
       </c>
       <c r="V12" s="8">
         <f t="shared" si="0"/>
-        <v>377.02011786766684</v>
+        <v>326.8324886150549</v>
       </c>
       <c r="W12" s="8">
         <f t="shared" si="0"/>
-        <v>386.96901955531752</v>
+        <v>335.45702652022504</v>
       </c>
       <c r="X12" s="8">
         <f t="shared" si="0"/>
-        <v>415.17199303509244</v>
+        <v>359.90571658183768</v>
       </c>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.45">
@@ -3006,31 +3006,31 @@
       </c>
       <c r="R16" s="6">
         <f>$Q$10*G16/SUM($G$16:$G$18)</f>
-        <v>18.282909188320392</v>
+        <v>15.849150817037239</v>
       </c>
       <c r="S16" s="6">
         <f>R16</f>
-        <v>18.282909188320392</v>
+        <v>15.849150817037239</v>
       </c>
       <c r="T16" s="6">
         <f t="shared" ref="T16:X16" si="2">S16</f>
-        <v>18.282909188320392</v>
+        <v>15.849150817037239</v>
       </c>
       <c r="U16" s="6">
         <f t="shared" si="2"/>
-        <v>18.282909188320392</v>
+        <v>15.849150817037239</v>
       </c>
       <c r="V16" s="6">
         <f t="shared" si="2"/>
-        <v>18.282909188320392</v>
+        <v>15.849150817037239</v>
       </c>
       <c r="W16" s="6">
         <f t="shared" si="2"/>
-        <v>18.282909188320392</v>
+        <v>15.849150817037239</v>
       </c>
       <c r="X16" s="6">
         <f t="shared" si="2"/>
-        <v>18.282909188320392</v>
+        <v>15.849150817037239</v>
       </c>
       <c r="Y16" t="s">
         <v>11</v>
@@ -3073,31 +3073,31 @@
       </c>
       <c r="R17" s="6">
         <f>$Q$10*G17/SUM($G$16:$G$18)</f>
-        <v>196.6133672649344</v>
+        <v>170.44086793463705</v>
       </c>
       <c r="S17" s="6">
         <f t="shared" ref="S17:X18" si="3">R17*H17/G17</f>
-        <v>232.51592552906516</v>
+        <v>201.56420037503352</v>
       </c>
       <c r="T17" s="6">
         <f t="shared" si="3"/>
-        <v>275.1952718992768</v>
+        <v>238.56221805518354</v>
       </c>
       <c r="U17" s="6">
         <f t="shared" si="3"/>
-        <v>283.93300294669177</v>
+        <v>246.13681221537641</v>
       </c>
       <c r="V17" s="6">
         <f t="shared" si="3"/>
-        <v>291.37305116528267</v>
+        <v>252.58646664880794</v>
       </c>
       <c r="W17" s="6">
         <f t="shared" si="3"/>
-        <v>302.56196088936514</v>
+        <v>262.28594695954996</v>
       </c>
       <c r="X17" s="6">
         <f t="shared" si="3"/>
-        <v>322.31557728368603</v>
+        <v>279.41002946691668</v>
       </c>
       <c r="Y17" t="s">
         <v>11</v>
@@ -3137,31 +3137,31 @@
       </c>
       <c r="R18" s="6">
         <f>$Q$10*G18/SUM($G$16:$G$18)</f>
-        <v>108.05372354674527</v>
+        <v>93.669981248325755</v>
       </c>
       <c r="S18" s="6">
         <f t="shared" si="3"/>
-        <v>98.104821859094599</v>
+        <v>85.045443343155654</v>
       </c>
       <c r="T18" s="6">
         <f t="shared" si="3"/>
-        <v>91.760594695955021</v>
+        <v>79.545738012322531</v>
       </c>
       <c r="U18" s="6">
         <f t="shared" si="3"/>
-        <v>83.887985534422739</v>
+        <v>72.721103669970532</v>
       </c>
       <c r="V18" s="6">
         <f t="shared" si="3"/>
-        <v>76.851660862577049</v>
+        <v>66.621430484864732</v>
       </c>
       <c r="W18" s="6">
         <f t="shared" si="3"/>
-        <v>73.881409054379873</v>
+        <v>64.046568443611051</v>
       </c>
       <c r="X18" s="6">
         <f t="shared" si="3"/>
-        <v>74.169783016340759</v>
+        <v>64.296555049558009</v>
       </c>
       <c r="Y18" t="s">
         <v>11</v>
@@ -3180,27 +3180,27 @@
       </c>
       <c r="S19" s="6">
         <f t="shared" ref="S19:X19" si="4">$Q$10*H16/SUM($G$16:$G$18)-S16</f>
-        <v>-4.6139833913742336</v>
+        <v>-3.9997856951513544</v>
       </c>
       <c r="T19" s="6">
         <f t="shared" si="4"/>
-        <v>2.0186177337262272</v>
+        <v>1.7499062416287163</v>
       </c>
       <c r="U19" s="6">
         <f t="shared" si="4"/>
-        <v>-4.2390972408250764</v>
+        <v>-3.6748031074203062</v>
       </c>
       <c r="V19" s="6">
         <f t="shared" si="4"/>
-        <v>-9.4875033485132647</v>
+        <v>-8.2245593356549715</v>
       </c>
       <c r="W19" s="6">
         <f t="shared" si="4"/>
-        <v>-7.7572595767479289</v>
+        <v>-6.7246396999732152</v>
       </c>
       <c r="X19" s="6">
         <f t="shared" si="4"/>
-        <v>0.40372354674524047</v>
+        <v>0.34998124832574184</v>
       </c>
       <c r="Y19" t="s">
         <v>11</v>

</xml_diff>